<commit_message>
Modified OODP PPTs and highlighted portions of the text
</commit_message>
<xml_diff>
--- a/S4/Exam.xlsx
+++ b/S4/Exam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srivi\Documents\COLLEGE STUFF\ACADEMICS\S4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0B72F88E-4596-439A-B79B-236C8BD17577}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3FDE03C5-CD81-406F-99D4-8BA091F93AA2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{6EB00AA6-6031-4A7B-8598-4ACCC5303AEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="22">
   <si>
     <t>BE</t>
   </si>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>9:30 - 12:30</t>
+  </si>
+  <si>
+    <t>OODP 5</t>
+  </si>
+  <si>
+    <t>OS 6</t>
+  </si>
+  <si>
+    <t>PDD 5</t>
+  </si>
+  <si>
+    <t>OODP 6</t>
   </si>
 </sst>
 </file>
@@ -460,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97B01130-A1B2-491A-95DE-9EEF9E1C1695}">
-  <dimension ref="A1:E162"/>
+  <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -474,592 +486,564 @@
     <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4">
-        <v>43603</v>
+        <v>43611</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <f t="shared" ref="A2:A51" si="0">A1+1</f>
+        <v>43612</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="4">
+        <f t="shared" si="0"/>
+        <v>43613</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4">
+        <f t="shared" si="0"/>
+        <v>43614</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <f t="shared" si="0"/>
+        <v>43615</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <f t="shared" si="0"/>
+        <v>43616</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <f t="shared" si="0"/>
+        <v>43617</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
-        <f t="shared" ref="A2:A59" si="0">A1+1</f>
-        <v>43604</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <f t="shared" si="0"/>
+        <v>43618</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
-        <f t="shared" si="0"/>
-        <v>43605</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <f t="shared" si="0"/>
+        <v>43619</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
-        <f t="shared" si="0"/>
-        <v>43606</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <f t="shared" si="0"/>
+        <v>43620</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <f t="shared" si="0"/>
-        <v>43607</v>
-      </c>
-      <c r="B5" s="7" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <f t="shared" si="0"/>
+        <v>43621</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
-        <f t="shared" si="0"/>
-        <v>43608</v>
-      </c>
-      <c r="B6" s="7" t="s">
+    <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <f t="shared" si="0"/>
+        <v>43622</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
-        <f t="shared" si="0"/>
-        <v>43609</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="C12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <f t="shared" si="0"/>
+        <v>43623</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
-        <f t="shared" si="0"/>
-        <v>43610</v>
-      </c>
-      <c r="B8" s="7" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <f t="shared" si="0"/>
+        <v>43624</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
-        <f t="shared" si="0"/>
-        <v>43611</v>
-      </c>
-      <c r="B9" s="7" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <f t="shared" si="0"/>
+        <v>43625</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
-        <f t="shared" si="0"/>
-        <v>43612</v>
-      </c>
-      <c r="B10" s="7" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <f t="shared" si="0"/>
+        <v>43626</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
-        <f t="shared" si="0"/>
-        <v>43613</v>
-      </c>
-      <c r="B11" s="7" t="s">
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5">
+        <f t="shared" si="0"/>
+        <v>43627</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
-        <f t="shared" si="0"/>
-        <v>43614</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
-        <f t="shared" si="0"/>
-        <v>43615</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
-        <f t="shared" si="0"/>
-        <v>43616</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
-        <f t="shared" si="0"/>
-        <v>43617</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
-        <f t="shared" si="0"/>
-        <v>43618</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
-        <f t="shared" si="0"/>
-        <v>43619</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>15</v>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
-        <v>43620</v>
+        <v>43628</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <f t="shared" si="0"/>
-        <v>43621</v>
+        <v>43629</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <f t="shared" si="0"/>
-        <v>43622</v>
+        <v>43630</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <f t="shared" si="0"/>
-        <v>43623</v>
+        <v>43631</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
-        <v>43624</v>
+        <v>43632</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="4">
-        <f t="shared" si="0"/>
-        <v>43625</v>
-      </c>
-      <c r="B23" s="7" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="5">
+        <f t="shared" si="0"/>
+        <v>43633</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
-        <v>43626</v>
+        <v>43634</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
-        <v>43627</v>
+        <v>43635</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <f t="shared" si="0"/>
-        <v>43628</v>
+        <v>43636</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="4">
-        <f t="shared" si="0"/>
-        <v>43629</v>
-      </c>
-      <c r="B27" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="5">
-        <f t="shared" si="0"/>
-        <v>43630</v>
-      </c>
-      <c r="B28" s="8" t="s">
+    <row r="27" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="5">
+        <f t="shared" si="0"/>
+        <v>43637</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="C27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
+        <f t="shared" si="0"/>
+        <v>43638</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <f t="shared" si="0"/>
-        <v>43631</v>
+        <v>43639</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
-        <v>43632</v>
+        <v>43640</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="5">
-        <f t="shared" si="0"/>
-        <v>43633</v>
-      </c>
-      <c r="B31" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>17</v>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="4">
+        <f t="shared" si="0"/>
+        <v>43641</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
-        <v>43634</v>
+        <v>43642</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="4">
+        <f t="shared" si="0"/>
+        <v>43643</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="4">
+        <f t="shared" si="0"/>
+        <v>43644</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="4">
+        <f t="shared" si="0"/>
+        <v>43645</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="4">
+        <f t="shared" si="0"/>
+        <v>43646</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="4">
+        <f t="shared" si="0"/>
+        <v>43647</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="4">
+        <f t="shared" si="0"/>
+        <v>43648</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="5">
-        <f t="shared" si="0"/>
-        <v>43635</v>
-      </c>
-      <c r="B33" s="8" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="4">
+        <f t="shared" si="0"/>
+        <v>43649</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="4">
-        <f t="shared" si="0"/>
-        <v>43636</v>
-      </c>
-      <c r="B34" s="7" t="s">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="4">
+        <f t="shared" si="0"/>
+        <v>43650</v>
+      </c>
+      <c r="B40" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5">
-        <f t="shared" si="0"/>
-        <v>43637</v>
-      </c>
-      <c r="B35" s="8" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="4">
+        <f t="shared" si="0"/>
+        <v>43651</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="4">
-        <f t="shared" si="0"/>
-        <v>43638</v>
-      </c>
-      <c r="B36" s="7" t="s">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="4">
+        <f t="shared" si="0"/>
+        <v>43652</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="4">
-        <f t="shared" si="0"/>
-        <v>43639</v>
-      </c>
-      <c r="B37" s="7" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="4">
+        <f t="shared" si="0"/>
+        <v>43653</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="4">
-        <f t="shared" si="0"/>
-        <v>43640</v>
-      </c>
-      <c r="B38" s="7" t="s">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="4">
+        <f t="shared" si="0"/>
+        <v>43654</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="4">
-        <f t="shared" si="0"/>
-        <v>43641</v>
-      </c>
-      <c r="B39" s="7" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="4">
+        <f t="shared" si="0"/>
+        <v>43655</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="4">
-        <f t="shared" si="0"/>
-        <v>43642</v>
-      </c>
-      <c r="B40" s="7" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="4">
+        <f t="shared" si="0"/>
+        <v>43656</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="4">
-        <f t="shared" si="0"/>
-        <v>43643</v>
-      </c>
-      <c r="B41" s="7" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="4">
+        <f t="shared" si="0"/>
+        <v>43657</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="4">
-        <f t="shared" si="0"/>
-        <v>43644</v>
-      </c>
-      <c r="B42" s="7" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="4">
+        <f t="shared" si="0"/>
+        <v>43658</v>
+      </c>
+      <c r="B48" s="7" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="4">
-        <f t="shared" si="0"/>
-        <v>43645</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="4">
-        <f t="shared" si="0"/>
-        <v>43646</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="4">
-        <f t="shared" si="0"/>
-        <v>43647</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="4">
-        <f t="shared" si="0"/>
-        <v>43648</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="4">
-        <f t="shared" si="0"/>
-        <v>43649</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="4">
-        <f t="shared" si="0"/>
-        <v>43650</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <f t="shared" si="0"/>
-        <v>43651</v>
+        <v>43659</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <f t="shared" si="0"/>
-        <v>43652</v>
+        <v>43660</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <f t="shared" si="0"/>
-        <v>43653</v>
+        <v>43661</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="4">
-        <f t="shared" si="0"/>
-        <v>43654</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="A52" s="4"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="4">
-        <f t="shared" si="0"/>
-        <v>43655</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="A53" s="4"/>
+      <c r="B53" s="7"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="4">
-        <f t="shared" si="0"/>
-        <v>43656</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="A54" s="4"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="4">
-        <f t="shared" si="0"/>
-        <v>43657</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="A55" s="4"/>
+      <c r="B55" s="7"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="4">
-        <f t="shared" si="0"/>
-        <v>43658</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>8</v>
-      </c>
+      <c r="A56" s="4"/>
+      <c r="B56" s="7"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="4">
-        <f t="shared" si="0"/>
-        <v>43659</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="A57" s="4"/>
+      <c r="B57" s="7"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="4">
-        <f t="shared" si="0"/>
-        <v>43660</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="A58" s="4"/>
+      <c r="B58" s="7"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="4">
-        <f t="shared" si="0"/>
-        <v>43661</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="A59" s="4"/>
+      <c r="B59" s="7"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="4"/>
@@ -1440,38 +1424,6 @@
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" s="4"/>
       <c r="B154" s="7"/>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A155" s="4"/>
-      <c r="B155" s="7"/>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A156" s="4"/>
-      <c r="B156" s="7"/>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A157" s="4"/>
-      <c r="B157" s="7"/>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A158" s="4"/>
-      <c r="B158" s="7"/>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A159" s="4"/>
-      <c r="B159" s="7"/>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A160" s="4"/>
-      <c r="B160" s="7"/>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A161" s="4"/>
-      <c r="B161" s="7"/>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A162" s="4"/>
-      <c r="B162" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Edited OODP PPTs, added DB PPT
</commit_message>
<xml_diff>
--- a/S4/Exam.xlsx
+++ b/S4/Exam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srivi\Documents\COLLEGE STUFF\ACADEMICS\S4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3FDE03C5-CD81-406F-99D4-8BA091F93AA2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1EB0795E-38DB-482E-9CEF-14C7A25557E9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{6EB00AA6-6031-4A7B-8598-4ACCC5303AEA}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,7 +506,7 @@
         <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -518,7 +518,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Renamed OS PPTs; added OODP code and note
</commit_message>
<xml_diff>
--- a/S4/Exam.xlsx
+++ b/S4/Exam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srivi\Documents\COLLEGE STUFF\ACADEMICS\S4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1EB0795E-38DB-482E-9CEF-14C7A25557E9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E0657431-AB26-4CB7-90FE-76269A0C7406}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{6EB00AA6-6031-4A7B-8598-4ACCC5303AEA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="30">
   <si>
     <t>BE</t>
   </si>
@@ -91,6 +91,30 @@
   </si>
   <si>
     <t>OODP 6</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>PDD 4</t>
+  </si>
+  <si>
+    <t>Recent topics not done</t>
+  </si>
+  <si>
+    <t>1, 2</t>
+  </si>
+  <si>
+    <t>3, 4</t>
+  </si>
+  <si>
+    <t>5, 6</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
 </sst>
 </file>
@@ -475,7 +499,7 @@
   <dimension ref="A1:E154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,6 +520,9 @@
       <c r="C1" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
@@ -508,6 +535,12 @@
       <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
@@ -520,6 +553,9 @@
       <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
@@ -532,6 +568,9 @@
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
@@ -541,6 +580,9 @@
       <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
@@ -550,6 +592,9 @@
       <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
@@ -625,6 +670,9 @@
       <c r="B13" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
@@ -634,6 +682,9 @@
       <c r="B14" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
@@ -643,6 +694,9 @@
       <c r="B15" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
@@ -651,6 +705,9 @@
       </c>
       <c r="B16" s="7" t="s">
         <v>11</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">

</xml_diff>